<commit_message>
config thông tin trong các sheet
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/CẦN THƠ 8 - 2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/CẦN THƠ 8 - 2024.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V43"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,16 +529,6 @@
           <t>Phụ phẫu 2</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Công phụ phẫu 1</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>Công phụ phẫu 2</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -621,12 +611,6 @@
       <c r="T2" t="n">
         <v/>
       </c>
-      <c r="U2" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -705,12 +689,6 @@
       <c r="T3" t="n">
         <v/>
       </c>
-      <c r="U3" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -791,12 +769,6 @@
       <c r="T4" t="n">
         <v/>
       </c>
-      <c r="U4" t="n">
-        <v>100000</v>
-      </c>
-      <c r="V4" t="n">
-        <v>50000</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -877,12 +849,6 @@
       <c r="T5" t="n">
         <v/>
       </c>
-      <c r="U5" t="n">
-        <v>100000</v>
-      </c>
-      <c r="V5" t="n">
-        <v>50000</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -963,12 +929,6 @@
       <c r="T6" t="n">
         <v/>
       </c>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1047,12 +1007,6 @@
       <c r="T7" t="n">
         <v/>
       </c>
-      <c r="U7" t="n">
-        <v>100000</v>
-      </c>
-      <c r="V7" t="n">
-        <v>50000</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1133,12 +1087,6 @@
       <c r="T8" t="n">
         <v/>
       </c>
-      <c r="U8" t="n">
-        <v/>
-      </c>
-      <c r="V8" t="n">
-        <v/>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1217,12 +1165,6 @@
       <c r="T9" t="n">
         <v/>
       </c>
-      <c r="U9" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1303,12 +1245,6 @@
       <c r="T10" t="n">
         <v/>
       </c>
-      <c r="U10" t="n">
-        <v>100000</v>
-      </c>
-      <c r="V10" t="n">
-        <v>50000</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1389,12 +1325,6 @@
       <c r="T11" t="n">
         <v/>
       </c>
-      <c r="U11" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1475,12 +1405,6 @@
       <c r="T12" t="n">
         <v/>
       </c>
-      <c r="U12" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1557,12 +1481,6 @@
       <c r="T13" t="n">
         <v/>
       </c>
-      <c r="U13" t="n">
-        <v/>
-      </c>
-      <c r="V13" t="n">
-        <v/>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1641,12 +1559,6 @@
       <c r="T14" t="n">
         <v/>
       </c>
-      <c r="U14" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V14" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1723,12 +1635,6 @@
       <c r="T15" t="n">
         <v/>
       </c>
-      <c r="U15" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1807,12 +1713,6 @@
       <c r="T16" t="n">
         <v/>
       </c>
-      <c r="U16" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1893,12 +1793,6 @@
       <c r="T17" t="n">
         <v/>
       </c>
-      <c r="U17" t="n">
-        <v/>
-      </c>
-      <c r="V17" t="n">
-        <v/>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1977,12 +1871,6 @@
       <c r="T18" t="n">
         <v/>
       </c>
-      <c r="U18" t="n">
-        <v>0</v>
-      </c>
-      <c r="V18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2063,12 +1951,6 @@
       <c r="T19" t="n">
         <v/>
       </c>
-      <c r="U19" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2149,12 +2031,6 @@
       <c r="T20" t="n">
         <v/>
       </c>
-      <c r="U20" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2237,12 +2113,6 @@
       <c r="T21" t="n">
         <v/>
       </c>
-      <c r="U21" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V21" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2323,12 +2193,6 @@
       <c r="T22" t="n">
         <v/>
       </c>
-      <c r="U22" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2409,12 +2273,6 @@
       <c r="T23" t="n">
         <v/>
       </c>
-      <c r="U23" t="n">
-        <v>100000</v>
-      </c>
-      <c r="V23" t="n">
-        <v>50000</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2493,12 +2351,6 @@
       <c r="T24" t="n">
         <v/>
       </c>
-      <c r="U24" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V24" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2577,12 +2429,6 @@
       <c r="T25" t="n">
         <v/>
       </c>
-      <c r="U25" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V25" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2661,12 +2507,6 @@
       <c r="T26" t="n">
         <v/>
       </c>
-      <c r="U26" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V26" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2749,12 +2589,6 @@
       <c r="T27" t="n">
         <v/>
       </c>
-      <c r="U27" t="n">
-        <v>100000</v>
-      </c>
-      <c r="V27" t="n">
-        <v>50000</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2833,12 +2667,6 @@
       <c r="T28" t="n">
         <v/>
       </c>
-      <c r="U28" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V28" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2919,12 +2747,6 @@
       <c r="T29" t="n">
         <v/>
       </c>
-      <c r="U29" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V29" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3003,12 +2825,6 @@
       <c r="T30" t="n">
         <v/>
       </c>
-      <c r="U30" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V30" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3087,12 +2903,6 @@
       <c r="T31" t="n">
         <v/>
       </c>
-      <c r="U31" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V31" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3173,12 +2983,6 @@
       <c r="T32" t="n">
         <v/>
       </c>
-      <c r="U32" t="n">
-        <v>100000</v>
-      </c>
-      <c r="V32" t="n">
-        <v>50000</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3257,12 +3061,6 @@
       <c r="T33" t="n">
         <v/>
       </c>
-      <c r="U33" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V33" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3341,12 +3139,6 @@
       <c r="T34" t="n">
         <v/>
       </c>
-      <c r="U34" t="n">
-        <v/>
-      </c>
-      <c r="V34" t="n">
-        <v/>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3427,12 +3219,6 @@
       <c r="T35" t="n">
         <v/>
       </c>
-      <c r="U35" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V35" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3511,12 +3297,6 @@
       <c r="T36" t="n">
         <v/>
       </c>
-      <c r="U36" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V36" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3595,12 +3375,6 @@
       <c r="T37" t="n">
         <v/>
       </c>
-      <c r="U37" t="n">
-        <v>0</v>
-      </c>
-      <c r="V37" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3681,12 +3455,6 @@
       <c r="T38" t="n">
         <v/>
       </c>
-      <c r="U38" t="n">
-        <v>100000</v>
-      </c>
-      <c r="V38" t="n">
-        <v>50000</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3765,12 +3533,6 @@
       <c r="T39" t="n">
         <v/>
       </c>
-      <c r="U39" t="n">
-        <v/>
-      </c>
-      <c r="V39" t="n">
-        <v/>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3849,12 +3611,6 @@
       <c r="T40" t="n">
         <v/>
       </c>
-      <c r="U40" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V40" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3933,12 +3689,6 @@
       <c r="T41" t="n">
         <v/>
       </c>
-      <c r="U41" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V41" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4016,12 +3766,6 @@
       </c>
       <c r="T42" t="n">
         <v/>
-      </c>
-      <c r="U42" t="n">
-        <v>50000</v>
-      </c>
-      <c r="V42" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -4065,12 +3809,6 @@
       </c>
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
-      <c r="U43" t="n">
-        <v>2000000</v>
-      </c>
-      <c r="V43" t="n">
-        <v>400000</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4083,7 +3821,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4149,37 +3887,17 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Đơn giá gốc</t>
+          <t>Đơn giá</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Sale phụ</t>
+          <t>Đã thanh toán</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Upsale</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Thanh toán lần đầu</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Đã thanh toán</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Bác sĩ 1</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Bác sĩ 2</t>
+          <t>Dư nợ</t>
         </is>
       </c>
     </row>
@@ -4239,24 +3957,10 @@
         <v>40000000</v>
       </c>
       <c r="M2" t="n">
-        <v/>
+        <v>40000000</v>
       </c>
       <c r="N2" t="n">
-        <v/>
-      </c>
-      <c r="O2" t="n">
-        <v>25000000</v>
-      </c>
-      <c r="P2" t="n">
-        <v>40000000</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R2" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -4315,24 +4019,10 @@
         <v>9000000</v>
       </c>
       <c r="M3" t="n">
-        <v/>
+        <v>4000000</v>
       </c>
       <c r="N3" t="n">
-        <v/>
-      </c>
-      <c r="O3" t="n">
-        <v/>
-      </c>
-      <c r="P3" t="n">
-        <v>4000000</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R3" t="n">
-        <v/>
+        <v>5000000</v>
       </c>
     </row>
     <row r="4">
@@ -4391,24 +4081,10 @@
         <v>20000000</v>
       </c>
       <c r="M4" t="n">
-        <v/>
+        <v>20000000</v>
       </c>
       <c r="N4" t="n">
-        <v/>
-      </c>
-      <c r="O4" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="P4" t="n">
-        <v>20000000</v>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Phạm Thanh Hoàng</t>
-        </is>
-      </c>
-      <c r="R4" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -4464,29 +4140,13 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Đỗ Thị Huyền Trân</t>
-        </is>
+        <v>18000000</v>
+      </c>
+      <c r="M5" t="n">
+        <v>12000000</v>
       </c>
       <c r="N5" t="n">
-        <v>8000000</v>
-      </c>
-      <c r="O5" t="n">
-        <v>9500000</v>
-      </c>
-      <c r="P5" t="n">
-        <v>12000000</v>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R5" t="n">
-        <v/>
+        <v>6000000</v>
       </c>
     </row>
     <row r="6">
@@ -4545,24 +4205,10 @@
         <v>15000000</v>
       </c>
       <c r="M6" t="n">
-        <v/>
+        <v>7000000</v>
       </c>
       <c r="N6" t="n">
-        <v/>
-      </c>
-      <c r="O6" t="n">
-        <v>5000000</v>
-      </c>
-      <c r="P6" t="n">
-        <v>7000000</v>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>Phạm Thanh Hoàng</t>
-        </is>
-      </c>
-      <c r="R6" t="n">
-        <v/>
+        <v>8000000</v>
       </c>
     </row>
     <row r="7">
@@ -4621,26 +4267,10 @@
         <v>20000000</v>
       </c>
       <c r="M7" t="n">
-        <v/>
+        <v>18000000</v>
       </c>
       <c r="N7" t="n">
-        <v/>
-      </c>
-      <c r="O7" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="P7" t="n">
-        <v>18000000</v>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>Phạm Thanh Hoàng</t>
-        </is>
+        <v>2000000</v>
       </c>
     </row>
     <row r="8">
@@ -4699,24 +4329,10 @@
         <v>35000000</v>
       </c>
       <c r="M8" t="n">
-        <v/>
+        <v>35000000</v>
       </c>
       <c r="N8" t="n">
-        <v/>
-      </c>
-      <c r="O8" t="n">
-        <v>32000000</v>
-      </c>
-      <c r="P8" t="n">
-        <v>35000000</v>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Phạm Thanh Hoàng</t>
-        </is>
-      </c>
-      <c r="R8" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -4775,24 +4391,10 @@
         <v>9000000</v>
       </c>
       <c r="M9" t="n">
-        <v/>
+        <v>8000000</v>
       </c>
       <c r="N9" t="n">
-        <v/>
-      </c>
-      <c r="O9" t="n">
-        <v>4000000</v>
-      </c>
-      <c r="P9" t="n">
-        <v>8000000</v>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R9" t="n">
-        <v/>
+        <v>1000000</v>
       </c>
     </row>
     <row r="10">
@@ -4851,24 +4453,10 @@
         <v>15000000</v>
       </c>
       <c r="M10" t="n">
-        <v/>
+        <v>15000000</v>
       </c>
       <c r="N10" t="n">
-        <v/>
-      </c>
-      <c r="O10" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="P10" t="n">
-        <v>15000000</v>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Phạm Thanh Hoàng</t>
-        </is>
-      </c>
-      <c r="R10" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -4927,24 +4515,10 @@
         <v>13000000</v>
       </c>
       <c r="M11" t="n">
-        <v/>
+        <v>13000000</v>
       </c>
       <c r="N11" t="n">
-        <v/>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>13000000</v>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>Nguyễn Hoàng Yến Quyên</t>
-        </is>
-      </c>
-      <c r="R11" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -5000,29 +4574,13 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>Đỗ Thị Huyền Trân</t>
-        </is>
+        <v>6000000</v>
+      </c>
+      <c r="M12" t="n">
+        <v>6000000</v>
       </c>
       <c r="N12" t="n">
-        <v>6000000</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>6000000</v>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>Nguyễn Hoàng Yến Quyên</t>
-        </is>
-      </c>
-      <c r="R12" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -5081,26 +4639,10 @@
         <v>20000000</v>
       </c>
       <c r="M13" t="n">
-        <v/>
+        <v>18000000</v>
       </c>
       <c r="N13" t="n">
-        <v/>
-      </c>
-      <c r="O13" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="P13" t="n">
-        <v>18000000</v>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>Phạm Thanh Hoàng</t>
-        </is>
+        <v>2000000</v>
       </c>
     </row>
     <row r="14">
@@ -5156,29 +4698,13 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Đỗ Thị Huyền Trân</t>
-        </is>
+        <v>18000000</v>
+      </c>
+      <c r="M14" t="n">
+        <v>12000000</v>
       </c>
       <c r="N14" t="n">
-        <v>8000000</v>
-      </c>
-      <c r="O14" t="n">
-        <v>9500000</v>
-      </c>
-      <c r="P14" t="n">
-        <v>12000000</v>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R14" t="n">
-        <v/>
+        <v>6000000</v>
       </c>
     </row>
     <row r="15">
@@ -5237,24 +4763,10 @@
         <v>9000000</v>
       </c>
       <c r="M15" t="n">
-        <v/>
+        <v>8000000</v>
       </c>
       <c r="N15" t="n">
-        <v/>
-      </c>
-      <c r="O15" t="n">
-        <v>4000000</v>
-      </c>
-      <c r="P15" t="n">
-        <v>8000000</v>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R15" t="n">
-        <v/>
+        <v>1000000</v>
       </c>
     </row>
     <row r="16">
@@ -5313,24 +4825,10 @@
         <v>9000000</v>
       </c>
       <c r="M16" t="n">
-        <v/>
+        <v>8000000</v>
       </c>
       <c r="N16" t="n">
-        <v/>
-      </c>
-      <c r="O16" t="n">
-        <v>4000000</v>
-      </c>
-      <c r="P16" t="n">
-        <v>8000000</v>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R16" t="n">
-        <v/>
+        <v>1000000</v>
       </c>
     </row>
     <row r="17">
@@ -5389,24 +4887,10 @@
         <v>25000000</v>
       </c>
       <c r="M17" t="n">
-        <v/>
+        <v>18800000</v>
       </c>
       <c r="N17" t="n">
-        <v/>
-      </c>
-      <c r="O17" t="n">
-        <v>2000000</v>
-      </c>
-      <c r="P17" t="n">
-        <v>18800000</v>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>Phạm Thanh Hoàng</t>
-        </is>
-      </c>
-      <c r="R17" t="n">
-        <v/>
+        <v>6200000</v>
       </c>
     </row>
     <row r="18">
@@ -5465,24 +4949,10 @@
         <v>38000000</v>
       </c>
       <c r="M18" t="n">
-        <v/>
+        <v>22000000</v>
       </c>
       <c r="N18" t="n">
-        <v/>
-      </c>
-      <c r="O18" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="P18" t="n">
-        <v>22000000</v>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>Lâm Thị Mỹ Hằng</t>
-        </is>
-      </c>
-      <c r="R18" t="n">
-        <v/>
+        <v>16000000</v>
       </c>
     </row>
     <row r="19">
@@ -5506,20 +4976,14 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="n">
-        <v>297000000</v>
-      </c>
-      <c r="M19" t="inlineStr"/>
+        <v>319000000</v>
+      </c>
+      <c r="M19" t="n">
+        <v>264800000</v>
+      </c>
       <c r="N19" t="n">
-        <v>22000000</v>
-      </c>
-      <c r="O19" t="n">
-        <v>145000000</v>
-      </c>
-      <c r="P19" t="n">
-        <v>264800000</v>
-      </c>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
+        <v>54200000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>